<commit_message>
Shopping af BMS done - skal sendes til Carl
</commit_message>
<xml_diff>
--- a/Documents/Shopping/BMS Shopping/Komponenter til rådighed BMS.xlsx
+++ b/Documents/Shopping/BMS Shopping/Komponenter til rådighed BMS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
   <si>
     <t>Antal</t>
   </si>
@@ -53,9 +53,6 @@
     <t>SN74AUP1G14 (DBVT)</t>
   </si>
   <si>
-    <t>BAV19W</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/panasonic-electronic-components/erja1aj270u/resistor-wide-term-27r-1-33w-5/dp/1670314</t>
   </si>
   <si>
@@ -435,6 +432,57 @@
   </si>
   <si>
     <t>Komponenter til rådighed BMS / INDKØB</t>
+  </si>
+  <si>
+    <t>MH 5 /Der er bestilt 5 stks BAV20W</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/diodes-inc/bav20w/diode-ss-150v-0-2a-sod123/dp/1902417</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/nxp/pmv37en/mosfet-n-ch-30v-3-1a-sot23/dp/1972682</t>
+  </si>
+  <si>
+    <t>MH 30 /Der er bestilt 5 stks PMV37EN</t>
+  </si>
+  <si>
+    <t>PMV90EN ##PMV37EN</t>
+  </si>
+  <si>
+    <t>BAV19W ##BAV20W</t>
+  </si>
+  <si>
+    <t>FM25V20-G ## FM25W256-G</t>
+  </si>
+  <si>
+    <t>MH 2 /Der er bestilt 2 stkFM25W256-G</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/cypress-semiconductor/fm25w256-g/fram-256k-spi-8soic/dp/2077756</t>
+  </si>
+  <si>
+    <t>SMD FUSE</t>
+  </si>
+  <si>
+    <t>FUSE</t>
+  </si>
+  <si>
+    <t>FRAM IC</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>USB-UART</t>
+  </si>
+  <si>
+    <t>KIT</t>
+  </si>
+  <si>
+    <t>MH 5 /købt slow acting</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/bourns/sf-0603s050-2/fuse-500ma-50vdc-smd-slow-blow/dp/2291892</t>
   </si>
 </sst>
 </file>
@@ -856,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,7 +916,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -878,7 +926,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -896,10 +944,10 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -925,7 +973,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -939,15 +987,15 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -956,15 +1004,18 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="G8" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -973,363 +1024,363 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28">
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29">
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1338,18 +1389,18 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="X31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32">
         <v>22</v>
@@ -1358,43 +1409,43 @@
         <v>6</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33">
         <v>45</v>
       </c>
       <c r="C33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
         <v>79</v>
       </c>
-      <c r="D33" t="s">
-        <v>80</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -1403,88 +1454,91 @@
         <v>6</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" t="s">
         <v>129</v>
       </c>
-      <c r="D40" t="s">
-        <v>130</v>
-      </c>
       <c r="E40" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1493,135 +1547,198 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="D44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
+      <c r="C45" t="s">
+        <v>150</v>
+      </c>
       <c r="D45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>135</v>
-      </c>
-      <c r="D46" t="s">
-        <v>108</v>
+        <v>134</v>
+      </c>
+      <c r="C46" t="s">
+        <v>107</v>
       </c>
       <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" t="s">
+        <v>139</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="C49" t="s">
+        <v>148</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" t="s">
+        <v>143</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>146</v>
+      </c>
+      <c r="D52" t="s">
+        <v>151</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1670,11 +1787,14 @@
     <hyperlink ref="E44" r:id="rId38"/>
     <hyperlink ref="E40" r:id="rId39"/>
     <hyperlink ref="E8" r:id="rId40"/>
+    <hyperlink ref="E47" r:id="rId41"/>
+    <hyperlink ref="E50" r:id="rId42"/>
+    <hyperlink ref="E52" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId44"/>
   <tableParts count="1">
-    <tablePart r:id="rId42"/>
+    <tablePart r:id="rId45"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>